<commit_message>
remove obsolete columns from data
</commit_message>
<xml_diff>
--- a/RToolbox/data/clementines_2019.xlsx
+++ b/RToolbox/data/clementines_2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\tutorials\MHSE-Statist\exercises\05d-Clementines-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\packages\Github\tpetzoldt\tpetzoldt.github.io\RToolbox\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBA9396-41A9-4453-BC99-BD75B8167744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7B5207-9ED8-49CB-A633-24D60775E6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="28">
   <si>
     <t>brand</t>
   </si>
@@ -35,12 +35,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>origin</t>
-  </si>
-  <si>
-    <t>package</t>
-  </si>
-  <si>
     <t>kilogram</t>
   </si>
   <si>
@@ -68,12 +62,6 @@
     <t>Basic</t>
   </si>
   <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Net</t>
-  </si>
-  <si>
     <t>EP</t>
   </si>
   <si>
@@ -117,19 +105,13 @@
   </si>
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -149,12 +131,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -179,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -187,7 +163,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -434,15 +409,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3828125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="14.15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,281 +428,200 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H2" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="I2" s="3">
-        <v>2.99</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.75</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5">
+        <v>2019</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1</v>
+      </c>
+      <c r="G9" s="3">
         <v>1.49</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H6" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="I6" s="3">
-        <v>2.99</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H7" s="3">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <v>2.29</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H8" s="3">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="5">
-        <v>2019</v>
-      </c>
-      <c r="H9" s="3">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3">
-        <v>1.49</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -756,22 +650,22 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -782,7 +676,7 @@
         <v>2019</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>107</v>
@@ -805,7 +699,7 @@
         <v>2019</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2">
         <v>100</v>
@@ -828,7 +722,7 @@
         <v>2019</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
         <v>89</v>
@@ -851,7 +745,7 @@
         <v>2019</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>99</v>
@@ -874,7 +768,7 @@
         <v>2019</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
         <v>99</v>
@@ -897,7 +791,7 @@
         <v>2019</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2">
         <v>96</v>
@@ -920,7 +814,7 @@
         <v>2019</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2">
         <v>100</v>
@@ -943,7 +837,7 @@
         <v>2019</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
         <v>89</v>
@@ -966,7 +860,7 @@
         <v>2019</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2">
         <v>86</v>
@@ -989,7 +883,7 @@
         <v>2019</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2">
         <v>92</v>
@@ -1012,7 +906,7 @@
         <v>2019</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2">
         <v>102</v>
@@ -1035,7 +929,7 @@
         <v>2019</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2">
         <v>92</v>
@@ -1058,7 +952,7 @@
         <v>2019</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2">
         <v>96</v>
@@ -1081,7 +975,7 @@
         <v>2019</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2">
         <v>90</v>
@@ -1104,7 +998,7 @@
         <v>2019</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2">
         <v>88</v>
@@ -1127,7 +1021,7 @@
         <v>2019</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2">
         <v>81</v>
@@ -1150,7 +1044,7 @@
         <v>2019</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2">
         <v>80</v>
@@ -1173,7 +1067,7 @@
         <v>2019</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2">
         <v>80</v>
@@ -1196,7 +1090,7 @@
         <v>2019</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D20" s="2">
         <v>75</v>
@@ -1219,7 +1113,7 @@
         <v>2019</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D21" s="2">
         <v>98</v>
@@ -1242,7 +1136,7 @@
         <v>2019</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D22" s="2">
         <v>82</v>
@@ -1265,7 +1159,7 @@
         <v>2019</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D23" s="2">
         <v>96</v>
@@ -1288,7 +1182,7 @@
         <v>2019</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D24" s="2">
         <v>81</v>
@@ -1311,7 +1205,7 @@
         <v>2019</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D25" s="2">
         <v>81</v>
@@ -1334,7 +1228,7 @@
         <v>2019</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2">
         <v>73</v>
@@ -1357,7 +1251,7 @@
         <v>2019</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D27" s="2">
         <v>87</v>
@@ -1380,7 +1274,7 @@
         <v>2019</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2">
         <v>72</v>
@@ -1403,7 +1297,7 @@
         <v>2019</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D29" s="2">
         <v>74</v>
@@ -1426,7 +1320,7 @@
         <v>2019</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D30" s="2">
         <v>75</v>
@@ -1449,7 +1343,7 @@
         <v>2019</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D31" s="2">
         <v>73</v>
@@ -1472,7 +1366,7 @@
         <v>2019</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D32" s="2">
         <v>65</v>
@@ -1495,7 +1389,7 @@
         <v>2019</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D33" s="2">
         <v>66</v>
@@ -1518,7 +1412,7 @@
         <v>2019</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2">
         <v>75</v>
@@ -1541,7 +1435,7 @@
         <v>2019</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D35" s="2">
         <v>92</v>
@@ -1564,7 +1458,7 @@
         <v>2019</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D36" s="2">
         <v>88</v>
@@ -1587,7 +1481,7 @@
         <v>2019</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D37" s="2">
         <v>93</v>
@@ -1610,7 +1504,7 @@
         <v>2019</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D38" s="2">
         <v>87</v>
@@ -1633,7 +1527,7 @@
         <v>2019</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D39" s="2">
         <v>88</v>
@@ -1656,7 +1550,7 @@
         <v>2019</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D40" s="2">
         <v>114</v>
@@ -1679,7 +1573,7 @@
         <v>2019</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D41" s="2">
         <v>74</v>
@@ -1702,7 +1596,7 @@
         <v>2019</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D42" s="2">
         <v>152</v>
@@ -1725,7 +1619,7 @@
         <v>2019</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D43" s="2">
         <v>113</v>
@@ -1748,7 +1642,7 @@
         <v>2019</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D44" s="2">
         <v>98</v>
@@ -1771,7 +1665,7 @@
         <v>2019</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D45" s="2">
         <v>125</v>
@@ -1794,7 +1688,7 @@
         <v>2019</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D46" s="2">
         <v>95</v>
@@ -1817,7 +1711,7 @@
         <v>2019</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D47" s="2">
         <v>109</v>
@@ -1840,7 +1734,7 @@
         <v>2019</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D48" s="2">
         <v>66</v>
@@ -1863,7 +1757,7 @@
         <v>2019</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D49" s="2">
         <v>118</v>
@@ -1886,7 +1780,7 @@
         <v>2019</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D50" s="2">
         <v>95</v>
@@ -1909,7 +1803,7 @@
         <v>2019</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D51" s="2">
         <v>120</v>
@@ -1932,7 +1826,7 @@
         <v>2019</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D52" s="2">
         <v>103</v>
@@ -1955,7 +1849,7 @@
         <v>2019</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D53" s="2">
         <v>64</v>
@@ -1978,7 +1872,7 @@
         <v>2019</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D54" s="2">
         <v>120</v>
@@ -2001,7 +1895,7 @@
         <v>2019</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D55" s="2">
         <v>114</v>
@@ -2024,7 +1918,7 @@
         <v>2019</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D56" s="2">
         <v>110</v>
@@ -2047,7 +1941,7 @@
         <v>2019</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D57" s="2">
         <v>115</v>
@@ -2070,7 +1964,7 @@
         <v>2019</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D58" s="2">
         <v>109</v>
@@ -2093,7 +1987,7 @@
         <v>2019</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D59" s="2">
         <v>101</v>
@@ -2116,7 +2010,7 @@
         <v>2019</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D60" s="2">
         <v>116</v>
@@ -2139,7 +2033,7 @@
         <v>2019</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D61" s="2">
         <v>110</v>

</xml_diff>